<commit_message>
now with updates from the TRB
</commit_message>
<xml_diff>
--- a/cagrid/Documentation/general/management/osu/trb/20110429 CaGrid TRB.xlsx
+++ b/cagrid/Documentation/general/management/osu/trb/20110429 CaGrid TRB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
   <si>
     <t xml:space="preserve">Tool </t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t> 03/29/11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TBD </t>
   </si>
   <si>
     <t>TBD</t>
@@ -203,28 +200,10 @@
     <t>Users on the Windows OS will need to manually move Introduce to a location with a less verbose path; this may just be a band-aid since adding more extensions to Introduce will increase the classpath further.</t>
   </si>
   <si>
-    <t>caGrid Introduce / caGrid Core Services</t>
-  </si>
-  <si>
-    <t>https://jira.citih.osumc.edu/browse/CAGRID-597</t>
-  </si>
-  <si>
-    <t>CAGRID-597</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
-    <t>Introduce generated clients  don't provide an obvious way to set the timeout when communicating with a remote service.  The default of 60s is not sufficient for users with long-running jobs (UAB's FQP use case)</t>
-  </si>
-  <si>
-    <t>The client code can be manually edited to facilitate setting the timeout, but users of the clent APIs in Jar format won't have this option.</t>
-  </si>
-  <si>
     <t>Low</t>
-  </si>
-  <si>
-    <t>The template that generates the client code should be trivial to update, but the upgrade tools to bring an existing service up to the latest version will need some attention to get this right.</t>
   </si>
   <si>
     <t>caGrid Dorian</t>
@@ -285,9 +264,6 @@
   </si>
   <si>
     <t>1.5-2.5 months of work remain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>We've been working on this since late last year.  Great progress has been made, and we're reasonably sure of the functionality.  Our security architect reports that the development grid we've deployed internally for testing is almost 100% functional, however some integration tests remain broken and are being investigated.  A community announcement regarding these changes and their impact on the community is still required, and the issue has been raised to EST (https://tracker.nci.nih.gov/browse/CSS-4)</t>
@@ -366,6 +342,27 @@
   </si>
   <si>
     <t>Related to CAGRID-652, it's important to know at what point the SDK data services are failing and figure out in which component the problem lies and if it's an easy fix</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Publish an erata on it for the Dorian administrators and leave it un-done for the moment.  It's an annoyance, rather than a functional problem.</t>
+  </si>
+  <si>
+    <t>Is open JDK even going to be an "allowed" part of the tech stack?</t>
+  </si>
+  <si>
+    <t>No action yet - see what community at large thinks and needs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Go</t>
+  </si>
+  <si>
+    <t>Pending SDK bug fix</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -849,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -865,7 +862,7 @@
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.140625" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" customWidth="1"/>
     <col min="13" max="13" width="16.85546875" customWidth="1"/>
     <col min="14" max="14" width="57.5703125" customWidth="1"/>
@@ -917,472 +914,431 @@
     </row>
     <row r="2" spans="1:14" ht="204.75" thickBot="1">
       <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="153.75" thickBot="1">
       <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="77.25" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="I4" s="16">
         <v>40662</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="115.5" thickBot="1">
       <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
       <c r="F5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="179.25" thickBot="1">
       <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="4"/>
       <c r="F6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="90" thickBot="1">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="4"/>
       <c r="F7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="191.25">
       <c r="A8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="I8" s="12">
         <v>40637</v>
       </c>
       <c r="J8" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="M8" s="9" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="204">
+    <row r="9" spans="1:14" ht="409.5">
       <c r="A9" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="I9" s="12">
         <v>40637</v>
       </c>
       <c r="J9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="M9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="191.25">
+      <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="C10" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="409.5">
-      <c r="A10" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="I10" s="12">
         <v>40637</v>
       </c>
       <c r="J10" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="M10" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="191.25">
+    <row r="11" spans="1:14" ht="178.5">
       <c r="A11" s="8" t="s">
-        <v>46</v>
+        <v>33</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>69</v>
-      </c>
       <c r="H11" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I11" s="12">
         <v>40637</v>
       </c>
       <c r="J11" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="191.25">
+      <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N11" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="8"/>
-      <c r="C12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="B12" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="12">
+        <v>40662</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="N12" s="14"/>
     </row>
-    <row r="13" spans="1:14" ht="178.5">
+    <row r="13" spans="1:14" ht="127.5">
       <c r="A13" s="8" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="I13" s="12">
-        <v>40637</v>
+        <v>40662</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="191.25">
-      <c r="A14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I14" s="12">
-        <v>40662</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N14" s="14"/>
-    </row>
-    <row r="15" spans="1:14" ht="127.5">
-      <c r="A15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="H15" t="s">
-        <v>99</v>
-      </c>
-      <c r="I15" s="12">
-        <v>40662</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1395,9 +1351,9 @@
     <hyperlink ref="H9" r:id="rId6"/>
     <hyperlink ref="H10" r:id="rId7"/>
     <hyperlink ref="H11" r:id="rId8"/>
-    <hyperlink ref="H13" r:id="rId9"/>
-    <hyperlink ref="H3" r:id="rId10"/>
-    <hyperlink ref="H14" r:id="rId11"/>
+    <hyperlink ref="H3" r:id="rId9"/>
+    <hyperlink ref="H12" r:id="rId10"/>
+    <hyperlink ref="H13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>

</xml_diff>